<commit_message>
Changes for NetzwerkPraktikum1 Blatt 1-3
</commit_message>
<xml_diff>
--- a/NetzwerkeI_Aufgabe3.1a.xlsx
+++ b/NetzwerkeI_Aufgabe3.1a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\Netzwerke_I_Praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Host</t>
   </si>
@@ -93,6 +93,33 @@
   </si>
   <si>
     <t>vDSL</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Service Provider</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
+  </si>
+  <si>
+    <t>Telekom</t>
+  </si>
+  <si>
+    <t>Betriebssystem</t>
+  </si>
+  <si>
+    <t>Windows 10</t>
+  </si>
+  <si>
+    <t>Zeit</t>
+  </si>
+  <si>
+    <t>Netzwerkadapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIGABIT Ethernet </t>
   </si>
 </sst>
 </file>
@@ -151,10 +178,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -436,22 +464,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,7 +504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -498,7 +528,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -522,7 +552,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -546,7 +576,7 @@
         <v>76.25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -570,7 +600,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -594,7 +624,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -610,8 +640,14 @@
       <c r="E8" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>VARA(C2:F2)</f>
         <v>0</v>
@@ -628,8 +664,14 @@
       <c r="E9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>VARA(C3:F3)</f>
         <v>0.33333333333333331</v>
@@ -646,8 +688,14 @@
       <c r="E10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>VARA(C4:F4)</f>
         <v>1.5833333333333333</v>
@@ -664,8 +712,14 @@
       <c r="E11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>VARA(C5:F5)</f>
         <v>0.25</v>
@@ -682,8 +736,14 @@
       <c r="E12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>VARA(C6:F6)</f>
         <v>0</v>
@@ -699,6 +759,78 @@
       </c>
       <c r="E13">
         <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>